<commit_message>
cleaned up and commented
</commit_message>
<xml_diff>
--- a/Opgaveoverblik.xlsx
+++ b/Opgaveoverblik.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" codeName="Denne_projektmappe" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB900DD-970D-45D7-A7A8-2EA54EAA8721}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6156DEB-3F68-4D17-A11F-EA5AD72442A3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="88">
   <si>
     <t>#</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>Standby - Map generator skal først have taget højde for at tilføje collision boxes selv da det pt kun tager højde for aller første gang "mappet bliver lavet"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der er recharge time på skudene nu og skibet kan nu skyde til hver side. </t>
   </si>
 </sst>
 </file>
@@ -1452,7 +1455,7 @@
   <dimension ref="A1:O387"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1570,7 +1573,7 @@
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" s="28" t="str">
         <f ca="1">IF(I3-TODAY()&lt;0, "Ingen Deadline valgt", I3-TODAY())</f>
@@ -1845,6 +1848,12 @@
         <v>56</v>
       </c>
       <c r="I12" s="6"/>
+      <c r="J12" s="38">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="M12" s="28" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>Ingen Deadline valgt</v>
@@ -4749,7 +4758,7 @@
       </c>
       <c r="M2" s="28">
         <f ca="1">IF(I2-TODAY()&lt;0, "Ingen Deadline valgt", I2-TODAY())</f>
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="O2" s="14"/>
     </row>
@@ -4775,9 +4784,9 @@
       <c r="J3" s="4">
         <v>0.25</v>
       </c>
-      <c r="M3" s="28">
+      <c r="M3" s="28" t="str">
         <f ca="1">IF(I3-TODAY()&lt;0, "Ingen Deadline valgt", I3-TODAY())</f>
-        <v>3</v>
+        <v>Ingen Deadline valgt</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>